<commit_message>
Deploying to gh-pages from  @ 1365ae6593f0de17c24a136cf6ebe4b29f49842d 🚀
</commit_message>
<xml_diff>
--- a/2021-03-04.xlsx
+++ b/2021-03-04.xlsx
@@ -5,24 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projekte\Abt3_IQM-COVID19\Fachlich\Auswertungen\2021-03-04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projekte\Abt3_IQM-COVID19\Fachlich\Auswertungen\2021-03-05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5BA787-AFA1-4561-B14E-BDF09EF4E4A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769D86BC-31C8-4F21-82BB-0C0E207E2BC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" tabRatio="597" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="9" r:id="rId1"/>
-    <sheet name="Gesamt_bis_einschl_03.03.21" sheetId="12" r:id="rId2"/>
-    <sheet name="Indik_bis_einschl_03.03." sheetId="11" r:id="rId3"/>
+    <sheet name="Gesamt_bis_einschl_04.03.21" sheetId="12" r:id="rId2"/>
+    <sheet name="Indik_bis_einschl_04.03." sheetId="11" r:id="rId3"/>
     <sheet name="Impfungen_proTag" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Bundesländer001" localSheetId="1">Gesamt_bis_einschl_03.03.21!#REF!</definedName>
-    <definedName name="Bundesländer001" localSheetId="2">Indik_bis_einschl_03.03.!$G$2:$J$18</definedName>
-    <definedName name="Bundesländer001_1" localSheetId="1">Gesamt_bis_einschl_03.03.21!$D$3:$H$19</definedName>
-    <definedName name="Bundesländer001_1" localSheetId="2">Indik_bis_einschl_03.03.!$C$2:$F$18</definedName>
+    <definedName name="Bundesländer001" localSheetId="1">Gesamt_bis_einschl_04.03.21!#REF!</definedName>
+    <definedName name="Bundesländer001" localSheetId="2">Indik_bis_einschl_04.03.!$G$2:$J$18</definedName>
+    <definedName name="Bundesländer001_1" localSheetId="1">Gesamt_bis_einschl_04.03.21!$D$3:$H$19</definedName>
+    <definedName name="Bundesländer001_1" localSheetId="2">Indik_bis_einschl_04.03.!$C$2:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Bayern</t>
   </si>
@@ -219,25 +219,31 @@
     <t>AstraZeneca</t>
   </si>
   <si>
-    <t>Bund (Einsatzkräfte Bundeswehr, Bundespolizei)</t>
-  </si>
-  <si>
-    <t>Durchgeführte Impfungen bundesweit und nach Bundesland bis einschließlich 03.03.21 (Gesamt_bis_einschl_03.03.21)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst alle Impfungen, die bis einschließlich 03.03.21 durchgeführt und bis zum 04.03.21, 8:00 Uhr, dem RKI gemeldet wurden. Nachmeldungen und Datenkorrekturen aus zurückliegenden Tagen sind in der kumulativen Zahl der Impfungen enthalten. </t>
-  </si>
-  <si>
-    <t>Anzahl Impfungen nach Indikation bis einschließlich 03.03.21 (Indik_bis_einschl_03.03.21)</t>
-  </si>
-  <si>
-    <t>Datenstand: 04.03.2021, 8:00 Uhr</t>
+    <t>Datenstand: 05.03.2021, 8:00 Uhr</t>
+  </si>
+  <si>
+    <t>Durchgeführte Impfungen bundesweit und nach Bundesland bis einschließlich 04.03.21 (Gesamt_bis_einschl_04.03.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst alle Impfungen, die bis einschließlich 04.03.21 durchgeführt und bis zum 05.03.21, 8:00 Uhr, dem RKI gemeldet wurden. Nachmeldungen und Datenkorrekturen aus zurückliegenden Tagen sind in der kumulativen Zahl der Impfungen enthalten. </t>
+  </si>
+  <si>
+    <t>Anzahl Impfungen nach Indikation bis einschließlich 04.03.21 (Indik_bis_einschl_04.03.21)</t>
+  </si>
+  <si>
+    <t>Bund *</t>
+  </si>
+  <si>
+    <t>* Impfungen, die in den bundeseigenen Impfzentren aus dem Impfkontingent des Bundes durchgeführt wurden. Diese gehen in die Berechnung der Impfquote für Gesamtdeutschland mit ein und umfassen nur Angehörige des Bundes, die nach §§ 2, 3 und 4 Coronavirus-Impfverordnung geimpft wurden. Die Impfungen sind erfasst, die Impfdaten befinden sich in Abstimmung.</t>
+  </si>
+  <si>
+    <t>** Impfungen, die in den bundeseigenen Impfzentren aus dem Impfkontingent des Bundes durchgeführt wurden. Diese gehen in die Berechnung der Impfquote für Gesamtdeutschland mit ein und umfassen nur Angehörige des Bundes, die nach §§ 2, 3 und 4 Coronavirus-Impfverordnung geimpft wurden. Die Impfungen sind erfasst, die Impfdaten befinden sich in Abstimmung.</t>
+  </si>
+  <si>
+    <t>Bund **</t>
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unter "Bund (Einsatzkräfte Bundeswehr, Bundespolizei)" werden alle Impfungen aufgeführt, die von Impfzentren der Bundeswehr/Bundespolizei - unabhängig von deren Standort - gemeldet werden. Diese Impfungen gehen in die Berechnung der Impfquote für Gesamtdeutschland ein, eine separate Ausweisung der Impfquote für diese Gruppe kann aufgrund einer fehlenden Bezugspopulation jedoch nicht erfolgen. </t>
   </si>
 </sst>
 </file>
@@ -337,7 +343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,12 +390,6 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -688,26 +688,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -772,8 +774,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -823,7 +825,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001_1" fillFormulas="1" connectionId="2" xr16:uid="{85D177FD-4909-4AAF-B663-F45CEC25E8F5}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001" fillFormulas="1" connectionId="1" xr16:uid="{8C6643A4-82D3-4F11-ADE7-BA4132573BCB}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="13">
     <queryTableFields count="4">
       <queryTableField id="5" name="Fälle in den letzten 7 Tagen"/>
@@ -844,7 +846,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001" fillFormulas="1" connectionId="1" xr16:uid="{8C6643A4-82D3-4F11-ADE7-BA4132573BCB}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001_1" fillFormulas="1" connectionId="2" xr16:uid="{85D177FD-4909-4AAF-B663-F45CEC25E8F5}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="13">
     <queryTableFields count="4">
       <queryTableField id="5" name="Fälle in den letzten 7 Tagen"/>
@@ -1188,7 +1190,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,7 +1211,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -1312,16 +1314,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A1EB7E-F725-49E9-9B87-E64B6D1D2BBC}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:N24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" style="5"/>
     <col min="7" max="7" width="13" style="32" customWidth="1"/>
@@ -1425,40 +1427,40 @@
         <v>1</v>
       </c>
       <c r="C4" s="26">
-        <v>879933</v>
+        <v>912712</v>
       </c>
       <c r="D4" s="10">
-        <v>587809</v>
+        <v>612465</v>
       </c>
       <c r="E4" s="10">
-        <v>470983</v>
+        <v>481082</v>
       </c>
       <c r="F4" s="10">
-        <v>30803</v>
+        <v>31378</v>
       </c>
       <c r="G4" s="10">
-        <v>86023</v>
+        <v>100005</v>
       </c>
       <c r="H4" s="10">
-        <v>22516</v>
+        <v>23104</v>
       </c>
       <c r="I4" s="25">
-        <v>5.2953886141338762</v>
+        <v>5.5175068560629468</v>
       </c>
       <c r="J4" s="22">
-        <v>292124</v>
+        <v>300247</v>
       </c>
       <c r="K4" s="10">
-        <v>286137</v>
+        <v>294189</v>
       </c>
       <c r="L4" s="10">
-        <v>5987</v>
+        <v>6058</v>
       </c>
       <c r="M4" s="11">
-        <v>8815</v>
+        <v>7800</v>
       </c>
       <c r="N4" s="42">
-        <v>2.6316543358731228</v>
+        <v>2.7048319185787459</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1469,40 +1471,40 @@
         <v>0</v>
       </c>
       <c r="C5" s="27">
-        <v>1150129</v>
+        <v>1226788</v>
       </c>
       <c r="D5" s="15">
-        <v>767969</v>
+        <v>817841</v>
       </c>
       <c r="E5" s="15">
-        <v>636768</v>
+        <v>664247</v>
       </c>
       <c r="F5" s="15">
-        <v>26260</v>
+        <v>29593</v>
       </c>
       <c r="G5" s="15">
-        <v>104941</v>
+        <v>124001</v>
       </c>
       <c r="H5" s="16">
-        <v>2403</v>
+        <v>26745</v>
       </c>
       <c r="I5" s="17">
-        <v>5.8513096300520155</v>
+        <v>6.2312943870799087</v>
       </c>
       <c r="J5" s="23">
-        <v>382160</v>
+        <v>408947</v>
       </c>
       <c r="K5" s="15">
-        <v>371456</v>
+        <v>398001</v>
       </c>
       <c r="L5" s="15">
-        <v>10704</v>
+        <v>10946</v>
       </c>
       <c r="M5" s="16">
-        <v>2057</v>
+        <v>14845</v>
       </c>
       <c r="N5" s="17">
-        <v>2.9117535840908659</v>
+        <v>3.1158491023477271</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1513,40 +1515,40 @@
         <v>3</v>
       </c>
       <c r="C6" s="26">
-        <v>325169</v>
+        <v>333422</v>
       </c>
       <c r="D6" s="10">
-        <v>201025</v>
+        <v>207729</v>
       </c>
       <c r="E6" s="10">
-        <v>166199</v>
+        <v>170933</v>
       </c>
       <c r="F6" s="10">
-        <v>7723</v>
+        <v>8614</v>
       </c>
       <c r="G6" s="10">
-        <v>27103</v>
+        <v>28182</v>
       </c>
       <c r="H6" s="11">
-        <v>5839</v>
+        <v>6704</v>
       </c>
       <c r="I6" s="12">
-        <v>5.4782802301463613</v>
+        <v>5.6609758683152513</v>
       </c>
       <c r="J6" s="22">
-        <v>124144</v>
+        <v>125693</v>
       </c>
       <c r="K6" s="10">
-        <v>121162</v>
+        <v>122565</v>
       </c>
       <c r="L6" s="10">
-        <v>2982</v>
+        <v>3128</v>
       </c>
       <c r="M6" s="11">
-        <v>2090</v>
+        <v>1549</v>
       </c>
       <c r="N6" s="12">
-        <v>3.383139514444919</v>
+        <v>3.42535245351467</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1557,40 +1559,40 @@
         <v>2</v>
       </c>
       <c r="C7" s="27">
-        <v>194149</v>
+        <v>199522</v>
       </c>
       <c r="D7" s="15">
-        <v>117854</v>
+        <v>122669</v>
       </c>
       <c r="E7" s="15">
-        <v>89140</v>
+        <v>90030</v>
       </c>
       <c r="F7" s="15">
-        <v>4207</v>
+        <v>4215</v>
       </c>
       <c r="G7" s="15">
-        <v>24507</v>
+        <v>28424</v>
       </c>
       <c r="H7" s="16">
-        <v>4693</v>
+        <v>4619</v>
       </c>
       <c r="I7" s="17">
-        <v>4.6732355417141012</v>
+        <v>4.8641635469863314</v>
       </c>
       <c r="J7" s="23">
-        <v>76295</v>
+        <v>76853</v>
       </c>
       <c r="K7" s="15">
-        <v>74730</v>
+        <v>74916</v>
       </c>
       <c r="L7" s="15">
-        <v>1565</v>
+        <v>1937</v>
       </c>
       <c r="M7" s="16">
-        <v>432</v>
+        <v>558</v>
       </c>
       <c r="N7" s="17">
-        <v>3.0253067834360934</v>
+        <v>3.0474330195610997</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1601,40 +1603,40 @@
         <v>4</v>
       </c>
       <c r="C8" s="26">
-        <v>63688</v>
+        <v>65814</v>
       </c>
       <c r="D8" s="10">
-        <v>41743</v>
+        <v>43573</v>
       </c>
       <c r="E8" s="10">
-        <v>31490</v>
+        <v>32097</v>
       </c>
       <c r="F8" s="10">
-        <v>2169</v>
+        <v>2369</v>
       </c>
       <c r="G8" s="10">
-        <v>8084</v>
+        <v>9107</v>
       </c>
       <c r="H8" s="11">
-        <v>2149</v>
+        <v>1830</v>
       </c>
       <c r="I8" s="12">
-        <v>6.1278446040968753</v>
+        <v>6.3964873855332183</v>
       </c>
       <c r="J8" s="22">
-        <v>21945</v>
+        <v>22241</v>
       </c>
       <c r="K8" s="10">
-        <v>20692</v>
+        <v>20988</v>
       </c>
       <c r="L8" s="10">
         <v>1253</v>
       </c>
       <c r="M8" s="11">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="N8" s="12">
-        <v>3.2215113872243477</v>
+        <v>3.2649639901233409</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1645,40 +1647,40 @@
         <v>5</v>
       </c>
       <c r="C9" s="27">
-        <v>164851</v>
+        <v>169350</v>
       </c>
       <c r="D9" s="15">
-        <v>108141</v>
+        <v>111435</v>
       </c>
       <c r="E9" s="15">
-        <v>84001</v>
+        <v>85417</v>
       </c>
       <c r="F9" s="15">
-        <v>1807</v>
+        <v>2102</v>
       </c>
       <c r="G9" s="15">
-        <v>22333</v>
+        <v>23916</v>
       </c>
       <c r="H9" s="16">
-        <v>2911</v>
+        <v>3226</v>
       </c>
       <c r="I9" s="17">
-        <v>5.8541520842028678</v>
+        <v>6.0324709176274176</v>
       </c>
       <c r="J9" s="23">
-        <v>56710</v>
+        <v>57915</v>
       </c>
       <c r="K9" s="15">
-        <v>55998</v>
+        <v>57137</v>
       </c>
       <c r="L9" s="15">
-        <v>712</v>
+        <v>778</v>
       </c>
       <c r="M9" s="16">
-        <v>1448</v>
+        <v>1140</v>
       </c>
       <c r="N9" s="17">
-        <v>3.0699638869174932</v>
+        <v>3.1351958827513071</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1689,40 +1691,40 @@
         <v>15</v>
       </c>
       <c r="C10" s="26">
-        <v>473235</v>
+        <v>491410</v>
       </c>
       <c r="D10" s="10">
-        <v>321415</v>
+        <v>333542</v>
       </c>
       <c r="E10" s="10">
-        <v>281244</v>
+        <v>288122</v>
       </c>
       <c r="F10" s="10">
-        <v>10239</v>
+        <v>10999</v>
       </c>
       <c r="G10" s="10">
-        <v>29932</v>
+        <v>34421</v>
       </c>
       <c r="H10" s="11">
-        <v>11167</v>
+        <v>12185</v>
       </c>
       <c r="I10" s="12">
-        <v>5.1114966730703166</v>
+        <v>5.3043536341776827</v>
       </c>
       <c r="J10" s="22">
-        <v>151820</v>
+        <v>157868</v>
       </c>
       <c r="K10" s="10">
-        <v>151664</v>
+        <v>157711</v>
       </c>
       <c r="L10" s="10">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="M10" s="11">
-        <v>6164</v>
+        <v>5923</v>
       </c>
       <c r="N10" s="12">
-        <v>2.4144094858844034</v>
+        <v>2.5105914683019299</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1733,40 +1735,40 @@
         <v>6</v>
       </c>
       <c r="C11" s="28">
-        <v>139042</v>
+        <v>143261</v>
       </c>
       <c r="D11" s="15">
-        <v>87249</v>
+        <v>90329</v>
       </c>
       <c r="E11" s="15">
-        <v>76652</v>
+        <v>78981</v>
       </c>
       <c r="F11" s="15">
-        <v>4820</v>
+        <v>5175</v>
       </c>
       <c r="G11" s="15">
-        <v>5777</v>
+        <v>6173</v>
       </c>
       <c r="H11" s="16">
-        <v>3256</v>
+        <v>3024</v>
       </c>
       <c r="I11" s="17">
-        <v>5.4254672173656742</v>
+        <v>5.6169930690027847</v>
       </c>
       <c r="J11" s="23">
-        <v>51793</v>
+        <v>52932</v>
       </c>
       <c r="K11" s="15">
-        <v>50606</v>
+        <v>51745</v>
       </c>
       <c r="L11" s="15">
         <v>1187</v>
       </c>
       <c r="M11" s="16">
-        <v>1110</v>
+        <v>1147</v>
       </c>
       <c r="N11" s="17">
-        <v>3.2206813096885964</v>
+        <v>3.2915085645634887</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1777,40 +1779,40 @@
         <v>7</v>
       </c>
       <c r="C12" s="26">
-        <v>590841</v>
+        <v>618518</v>
       </c>
       <c r="D12" s="10">
-        <v>409203</v>
+        <v>431056</v>
       </c>
       <c r="E12" s="10">
-        <v>346798</v>
+        <v>361028</v>
       </c>
       <c r="F12" s="10">
-        <v>12628</v>
+        <v>14236</v>
       </c>
       <c r="G12" s="10">
-        <v>49777</v>
+        <v>55792</v>
       </c>
       <c r="H12" s="11">
-        <v>16082</v>
+        <v>19873</v>
       </c>
       <c r="I12" s="12">
-        <v>5.119127683018732</v>
+        <v>5.3925086143828915</v>
       </c>
       <c r="J12" s="22">
-        <v>181638</v>
+        <v>187462</v>
       </c>
       <c r="K12" s="10">
-        <v>179443</v>
+        <v>184582</v>
       </c>
       <c r="L12" s="10">
-        <v>2195</v>
+        <v>2880</v>
       </c>
       <c r="M12" s="11">
-        <v>4770</v>
+        <v>5407</v>
       </c>
       <c r="N12" s="12">
-        <v>2.272290560157566</v>
+        <v>2.3451487738703225</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1821,40 +1823,40 @@
         <v>8</v>
       </c>
       <c r="C13" s="27">
-        <v>1409038</v>
+        <v>1457675</v>
       </c>
       <c r="D13" s="15">
-        <v>959746</v>
+        <v>994848</v>
       </c>
       <c r="E13" s="15">
-        <v>794705</v>
+        <v>807163</v>
       </c>
       <c r="F13" s="15">
-        <v>21634</v>
+        <v>22300</v>
       </c>
       <c r="G13" s="15">
-        <v>143407</v>
+        <v>165385</v>
       </c>
       <c r="H13" s="16">
-        <v>33483</v>
+        <v>31210</v>
       </c>
       <c r="I13" s="17">
-        <v>5.3476022833841519</v>
+        <v>5.5431868811332965</v>
       </c>
       <c r="J13" s="23">
-        <v>449292</v>
+        <v>462827</v>
       </c>
       <c r="K13" s="15">
-        <v>442428</v>
+        <v>455135</v>
       </c>
       <c r="L13" s="15">
-        <v>6864</v>
+        <v>7692</v>
       </c>
       <c r="M13" s="16">
-        <v>14989</v>
+        <v>9638</v>
       </c>
       <c r="N13" s="17">
-        <v>2.5034070734405063</v>
+        <v>2.5788226489215238</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1865,40 +1867,40 @@
         <v>12</v>
       </c>
       <c r="C14" s="26">
-        <v>380545</v>
+        <v>391488</v>
       </c>
       <c r="D14" s="10">
-        <v>239974</v>
+        <v>250557</v>
       </c>
       <c r="E14" s="10">
-        <v>190300</v>
+        <v>192038</v>
       </c>
       <c r="F14" s="10">
         <v>4536</v>
       </c>
       <c r="G14" s="10">
-        <v>45138</v>
+        <v>53983</v>
       </c>
       <c r="H14" s="11">
-        <v>9540</v>
+        <v>10452</v>
       </c>
       <c r="I14" s="12">
-        <v>5.8617412283583663</v>
+        <v>6.1202475974638384</v>
       </c>
       <c r="J14" s="22">
-        <v>140571</v>
+        <v>140931</v>
       </c>
       <c r="K14" s="10">
-        <v>136840</v>
+        <v>137200</v>
       </c>
       <c r="L14" s="10">
         <v>3731</v>
       </c>
       <c r="M14" s="11">
-        <v>219</v>
+        <v>354</v>
       </c>
       <c r="N14" s="12">
-        <v>3.4336670898162462</v>
+        <v>3.4424606542949356</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1909,40 +1911,40 @@
         <v>13</v>
       </c>
       <c r="C15" s="27">
-        <v>84145</v>
+        <v>88170</v>
       </c>
       <c r="D15" s="15">
-        <v>59748</v>
+        <v>62931</v>
       </c>
       <c r="E15" s="15">
-        <v>45901</v>
+        <v>47498</v>
       </c>
       <c r="F15" s="15">
-        <v>1854</v>
+        <v>1992</v>
       </c>
       <c r="G15" s="15">
-        <v>11993</v>
+        <v>13441</v>
       </c>
       <c r="H15" s="16">
-        <v>3302</v>
+        <v>3189</v>
       </c>
       <c r="I15" s="17">
-        <v>6.0541885747811044</v>
+        <v>6.3767179018469191</v>
       </c>
       <c r="J15" s="23">
-        <v>24397</v>
+        <v>25239</v>
       </c>
       <c r="K15" s="15">
-        <v>23451</v>
+        <v>24182</v>
       </c>
       <c r="L15" s="15">
-        <v>946</v>
+        <v>1057</v>
       </c>
       <c r="M15" s="16">
-        <v>523</v>
+        <v>843</v>
       </c>
       <c r="N15" s="17">
-        <v>2.4721168684965957</v>
+        <v>2.5574356537273264</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1953,40 +1955,40 @@
         <v>9</v>
       </c>
       <c r="C16" s="26">
-        <v>338948</v>
+        <v>350765</v>
       </c>
       <c r="D16" s="10">
-        <v>235347</v>
+        <v>244306</v>
       </c>
       <c r="E16" s="10">
-        <v>211510</v>
+        <v>217891</v>
       </c>
       <c r="F16" s="10">
-        <v>11594</v>
+        <v>11995</v>
       </c>
       <c r="G16" s="10">
-        <v>12243</v>
+        <v>14420</v>
       </c>
       <c r="H16" s="11">
-        <v>8597</v>
+        <v>8959</v>
       </c>
       <c r="I16" s="12">
-        <v>5.7796826156178422</v>
+        <v>5.9996989173056487</v>
       </c>
       <c r="J16" s="22">
-        <v>103601</v>
+        <v>106459</v>
       </c>
       <c r="K16" s="10">
-        <v>102563</v>
+        <v>105114</v>
       </c>
       <c r="L16" s="10">
-        <v>1038</v>
+        <v>1345</v>
       </c>
       <c r="M16" s="11">
-        <v>2703</v>
+        <v>2858</v>
       </c>
       <c r="N16" s="12">
-        <v>2.5442469997944483</v>
+        <v>2.6144341401252613</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1997,40 +1999,40 @@
         <v>10</v>
       </c>
       <c r="C17" s="27">
-        <v>167937</v>
+        <v>174191</v>
       </c>
       <c r="D17" s="15">
-        <v>111342</v>
+        <v>115502</v>
       </c>
       <c r="E17" s="15">
-        <v>87410</v>
+        <v>89442</v>
       </c>
       <c r="F17" s="15">
-        <v>5498</v>
+        <v>6023</v>
       </c>
       <c r="G17" s="15">
-        <v>18434</v>
+        <v>20037</v>
       </c>
       <c r="H17" s="16">
-        <v>5013</v>
+        <v>4160</v>
       </c>
       <c r="I17" s="17">
-        <v>5.0730323102704507</v>
+        <v>5.262572774881515</v>
       </c>
       <c r="J17" s="23">
-        <v>56595</v>
+        <v>58689</v>
       </c>
       <c r="K17" s="15">
-        <v>55435</v>
+        <v>57215</v>
       </c>
       <c r="L17" s="15">
-        <v>1160</v>
+        <v>1474</v>
       </c>
       <c r="M17" s="16">
-        <v>1669</v>
+        <v>2094</v>
       </c>
       <c r="N17" s="17">
-        <v>2.5786160083324905</v>
+        <v>2.6740241172016175</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -2041,40 +2043,40 @@
         <v>11</v>
       </c>
       <c r="C18" s="26">
-        <v>255582</v>
+        <v>263163</v>
       </c>
       <c r="D18" s="10">
-        <v>162163</v>
+        <v>168238</v>
       </c>
       <c r="E18" s="10">
-        <v>131025</v>
+        <v>134424</v>
       </c>
       <c r="F18" s="10">
-        <v>4981</v>
+        <v>5207</v>
       </c>
       <c r="G18" s="10">
-        <v>26157</v>
+        <v>28607</v>
       </c>
       <c r="H18" s="11">
-        <v>6790</v>
+        <v>5969</v>
       </c>
       <c r="I18" s="12">
-        <v>5.584561878631698</v>
+        <v>5.7937724470886671</v>
       </c>
       <c r="J18" s="22">
-        <v>93419</v>
+        <v>94925</v>
       </c>
       <c r="K18" s="10">
-        <v>91979</v>
+        <v>93442</v>
       </c>
       <c r="L18" s="10">
-        <v>1440</v>
+        <v>1483</v>
       </c>
       <c r="M18" s="11">
-        <v>1180</v>
+        <v>1508</v>
       </c>
       <c r="N18" s="12">
-        <v>3.2171591925401879</v>
+        <v>3.2690227507453233</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -2085,136 +2087,124 @@
         <v>14</v>
       </c>
       <c r="C19" s="27">
-        <v>191564</v>
+        <v>196313</v>
       </c>
       <c r="D19" s="15">
-        <v>127282</v>
+        <v>129153</v>
       </c>
       <c r="E19" s="15">
-        <v>104352</v>
+        <v>105883</v>
       </c>
       <c r="F19" s="15">
-        <v>8320</v>
+        <v>8321</v>
       </c>
       <c r="G19" s="15">
-        <v>14610</v>
+        <v>14949</v>
       </c>
       <c r="H19" s="16">
-        <v>2423</v>
+        <v>1621</v>
       </c>
       <c r="I19" s="17">
-        <v>5.9662188322931993</v>
+        <v>6.0539201210474651</v>
       </c>
       <c r="J19" s="23">
-        <v>64282</v>
+        <v>67160</v>
       </c>
       <c r="K19" s="15">
-        <v>63748</v>
+        <v>66088</v>
       </c>
       <c r="L19" s="15">
-        <v>534</v>
+        <v>1072</v>
       </c>
       <c r="M19" s="16">
-        <v>2445</v>
+        <v>2893</v>
       </c>
       <c r="N19" s="17">
-        <v>3.0131556620533257</v>
+        <v>3.1480590875128547</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="26">
-        <v>4377</v>
-      </c>
-      <c r="D20" s="10">
-        <v>3379</v>
-      </c>
-      <c r="E20" s="10">
-        <v>2654</v>
-      </c>
-      <c r="F20" s="10">
-        <v>0</v>
-      </c>
-      <c r="G20" s="10">
-        <v>725</v>
-      </c>
-      <c r="H20" s="11">
-        <v>590</v>
+        <v>62</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="J20" s="22">
-        <v>998</v>
-      </c>
-      <c r="K20" s="10">
-        <v>997</v>
-      </c>
-      <c r="L20" s="10">
-        <v>0</v>
-      </c>
-      <c r="M20" s="11">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="44"/>
+      <c r="B21" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="45">
-        <f>D21+J21</f>
-        <v>6813173</v>
-      </c>
-      <c r="D21" s="46">
-        <f>SUM(D4:D20)</f>
-        <v>4541389</v>
-      </c>
-      <c r="E21" s="46">
-        <f>SUM(E4:E20)</f>
-        <v>3751132</v>
-      </c>
-      <c r="F21" s="46">
-        <f>SUM(F4:F20)</f>
-        <v>159073</v>
-      </c>
-      <c r="G21" s="46">
-        <f>SUM(G4:G20)</f>
-        <v>631184</v>
-      </c>
-      <c r="H21" s="46">
-        <f>SUM(H4:H20)</f>
-        <v>140754</v>
+      <c r="C21" s="46">
+        <v>7082562</v>
+      </c>
+      <c r="D21" s="44">
+        <v>4736174</v>
+      </c>
+      <c r="E21" s="44">
+        <v>3846276</v>
+      </c>
+      <c r="F21" s="44">
+        <v>169055</v>
+      </c>
+      <c r="G21" s="44">
+        <v>720843</v>
+      </c>
+      <c r="H21" s="44">
+        <v>166870</v>
       </c>
       <c r="I21" s="47">
-        <f>D21/83166711*100</f>
-        <v>5.4605850650989431</v>
+        <v>5.6947953610910496</v>
       </c>
       <c r="J21" s="48">
-        <f>SUM(J4:J20)</f>
-        <v>2271784</v>
-      </c>
-      <c r="K21" s="46">
-        <f>SUM(K4:K20)</f>
-        <v>2229329</v>
-      </c>
-      <c r="L21" s="46">
-        <f>SUM(L4:L20)</f>
-        <v>42454</v>
-      </c>
-      <c r="M21" s="46">
-        <f>SUM(M4:M20)</f>
-        <v>50938</v>
+        <v>2346388</v>
+      </c>
+      <c r="K21" s="44">
+        <v>2300210</v>
+      </c>
+      <c r="L21" s="44">
+        <v>46178</v>
+      </c>
+      <c r="M21" s="44">
+        <v>58853</v>
       </c>
       <c r="N21" s="47">
-        <f>J21/83166711*100</f>
-        <v>2.7316025518912248</v>
+        <v>2.8213067124898088</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2222,26 +2212,26 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="74"/>
-      <c r="L24" s="74"/>
-      <c r="M24" s="74"/>
-      <c r="N24" s="74"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C28" s="24"/>
+    <row r="24" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2262,7 +2252,6 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A4:A19" numberStoredAsText="1"/>
-    <ignoredError sqref="I21" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2271,14 +2260,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F4549C-7AD6-45E3-9E9E-50890FFA92FE}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.42578125" style="5"/>
     <col min="5" max="5" width="12.7109375" style="5" customWidth="1"/>
     <col min="6" max="6" width="13" style="5" customWidth="1"/>
@@ -2345,28 +2334,28 @@
         <v>1</v>
       </c>
       <c r="C3" s="13">
-        <v>318116</v>
+        <v>326233</v>
       </c>
       <c r="D3" s="11">
-        <v>226000</v>
+        <v>239847</v>
       </c>
       <c r="E3" s="11">
-        <v>18473</v>
+        <v>20117</v>
       </c>
       <c r="F3" s="14">
-        <v>81231</v>
+        <v>82117</v>
       </c>
       <c r="G3" s="13">
-        <v>166796</v>
+        <v>171774</v>
       </c>
       <c r="H3" s="11">
-        <v>104566</v>
+        <v>107212</v>
       </c>
       <c r="I3" s="11">
-        <v>7116</v>
+        <v>7363</v>
       </c>
       <c r="J3" s="14">
-        <v>56940</v>
+        <v>58292</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2377,28 +2366,28 @@
         <v>0</v>
       </c>
       <c r="C4" s="19">
-        <v>330441</v>
+        <v>354388</v>
       </c>
       <c r="D4" s="16">
-        <v>350733</v>
+        <v>370418</v>
       </c>
       <c r="E4" s="16">
-        <v>34410</v>
+        <v>40269</v>
       </c>
       <c r="F4" s="18">
-        <v>120145</v>
+        <v>122272</v>
       </c>
       <c r="G4" s="19">
-        <v>133217</v>
+        <v>148459</v>
       </c>
       <c r="H4" s="16">
-        <v>196457</v>
+        <v>205257</v>
       </c>
       <c r="I4" s="16">
-        <v>8075</v>
+        <v>8960</v>
       </c>
       <c r="J4" s="18">
-        <v>92233</v>
+        <v>95667</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2409,28 +2398,28 @@
         <v>3</v>
       </c>
       <c r="C5" s="13">
-        <v>137085</v>
+        <v>142291</v>
       </c>
       <c r="D5" s="11">
-        <v>64698</v>
+        <v>66478</v>
       </c>
       <c r="E5" s="11">
         <v>150</v>
       </c>
       <c r="F5" s="14">
-        <v>42669</v>
+        <v>42869</v>
       </c>
       <c r="G5" s="13">
-        <v>92942</v>
+        <v>94202</v>
       </c>
       <c r="H5" s="11">
-        <v>29559</v>
+        <v>29829</v>
       </c>
       <c r="I5" s="11">
         <v>30</v>
       </c>
       <c r="J5" s="14">
-        <v>34392</v>
+        <v>34809</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2441,28 +2430,28 @@
         <v>2</v>
       </c>
       <c r="C6" s="19">
-        <v>47459</v>
+        <v>48287</v>
       </c>
       <c r="D6" s="16">
-        <v>62913</v>
+        <v>66104</v>
       </c>
       <c r="E6" s="16">
-        <v>5063</v>
+        <v>5834</v>
       </c>
       <c r="F6" s="18">
-        <v>22125</v>
+        <v>22181</v>
       </c>
       <c r="G6" s="19">
-        <v>33911</v>
+        <v>34381</v>
       </c>
       <c r="H6" s="16">
-        <v>40841</v>
+        <v>40914</v>
       </c>
       <c r="I6" s="16">
-        <v>1098</v>
+        <v>1109</v>
       </c>
       <c r="J6" s="18">
-        <v>16930</v>
+        <v>17083</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2473,28 +2462,28 @@
         <v>4</v>
       </c>
       <c r="C7" s="13">
-        <v>18259</v>
+        <v>18850</v>
       </c>
       <c r="D7" s="11">
-        <v>19299</v>
+        <v>20474</v>
       </c>
       <c r="E7" s="11">
-        <v>727</v>
+        <v>886</v>
       </c>
       <c r="F7" s="14">
-        <v>8073</v>
+        <v>8079</v>
       </c>
       <c r="G7" s="13">
-        <v>10200</v>
+        <v>10424</v>
       </c>
       <c r="H7" s="11">
-        <v>8796</v>
+        <v>8855</v>
       </c>
       <c r="I7" s="11">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J7" s="14">
-        <v>6911</v>
+        <v>6917</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2505,28 +2494,28 @@
         <v>5</v>
       </c>
       <c r="C8" s="19">
-        <v>45736</v>
+        <v>47254</v>
       </c>
       <c r="D8" s="16">
-        <v>55391</v>
+        <v>57075</v>
       </c>
       <c r="E8" s="16">
-        <v>2011</v>
+        <v>2061</v>
       </c>
       <c r="F8" s="18">
-        <v>15740</v>
+        <v>15826</v>
       </c>
       <c r="G8" s="19">
-        <v>22465</v>
+        <v>23290</v>
       </c>
       <c r="H8" s="16">
-        <v>30722</v>
+        <v>31056</v>
       </c>
       <c r="I8" s="16">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="J8" s="18">
-        <v>12260</v>
+        <v>12361</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2537,28 +2526,28 @@
         <v>15</v>
       </c>
       <c r="C9" s="13">
-        <v>163751</v>
+        <v>168950</v>
       </c>
       <c r="D9" s="11">
-        <v>126850</v>
+        <v>134121</v>
       </c>
       <c r="E9" s="11">
-        <v>8202</v>
+        <v>8655</v>
       </c>
       <c r="F9" s="14">
-        <v>50731</v>
+        <v>49776</v>
       </c>
       <c r="G9" s="13">
-        <v>68241</v>
+        <v>72888</v>
       </c>
       <c r="H9" s="11">
-        <v>65602</v>
+        <v>66798</v>
       </c>
       <c r="I9" s="11">
-        <v>6034</v>
+        <v>6414</v>
       </c>
       <c r="J9" s="14">
-        <v>34410</v>
+        <v>34906</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2569,28 +2558,28 @@
         <v>6</v>
       </c>
       <c r="C10" s="19">
-        <v>28343</v>
+        <v>30535</v>
       </c>
       <c r="D10" s="16">
-        <v>35630</v>
+        <v>36325</v>
       </c>
       <c r="E10" s="16">
-        <v>1806</v>
+        <v>1876</v>
       </c>
       <c r="F10" s="18">
-        <v>24024</v>
+        <v>24379</v>
       </c>
       <c r="G10" s="19">
-        <v>11175</v>
+        <v>11847</v>
       </c>
       <c r="H10" s="16">
-        <v>25088</v>
+        <v>25490</v>
       </c>
       <c r="I10" s="16">
-        <v>662</v>
+        <v>671</v>
       </c>
       <c r="J10" s="18">
-        <v>15927</v>
+        <v>16142</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2601,28 +2590,28 @@
         <v>7</v>
       </c>
       <c r="C11" s="13">
-        <v>191568</v>
+        <v>206332</v>
       </c>
       <c r="D11" s="11">
-        <v>160292</v>
+        <v>166651</v>
       </c>
       <c r="E11" s="11">
-        <v>41090</v>
+        <v>42503</v>
       </c>
       <c r="F11" s="14">
-        <v>93864</v>
+        <v>94737</v>
       </c>
       <c r="G11" s="13">
-        <v>44146</v>
+        <v>47128</v>
       </c>
       <c r="H11" s="11">
-        <v>94449</v>
+        <v>96537</v>
       </c>
       <c r="I11" s="11">
-        <v>27653</v>
+        <v>28258</v>
       </c>
       <c r="J11" s="14">
-        <v>74007</v>
+        <v>75550</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2633,28 +2622,28 @@
         <v>8</v>
       </c>
       <c r="C12" s="19">
-        <v>323123</v>
+        <v>333595</v>
       </c>
       <c r="D12" s="16">
-        <v>505582</v>
+        <v>529027</v>
       </c>
       <c r="E12" s="16">
-        <v>18201</v>
+        <v>18787</v>
       </c>
       <c r="F12" s="18">
-        <v>185138</v>
+        <v>186154</v>
       </c>
       <c r="G12" s="19">
-        <v>77615</v>
+        <v>82883</v>
       </c>
       <c r="H12" s="16">
-        <v>276962</v>
+        <v>284118</v>
       </c>
       <c r="I12" s="16">
-        <v>13119</v>
+        <v>13508</v>
       </c>
       <c r="J12" s="18">
-        <v>142056</v>
+        <v>143759</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2665,28 +2654,28 @@
         <v>12</v>
       </c>
       <c r="C13" s="13">
-        <v>92431</v>
+        <v>94019</v>
       </c>
       <c r="D13" s="11">
-        <v>108418</v>
+        <v>116728</v>
       </c>
       <c r="E13" s="11">
-        <v>3155</v>
+        <v>3802</v>
       </c>
       <c r="F13" s="14">
-        <v>35970</v>
+        <v>36008</v>
       </c>
       <c r="G13" s="13">
-        <v>52267</v>
+        <v>52285</v>
       </c>
       <c r="H13" s="11">
-        <v>57100</v>
+        <v>57283</v>
       </c>
       <c r="I13" s="11">
         <v>90</v>
       </c>
       <c r="J13" s="14">
-        <v>31114</v>
+        <v>31273</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2697,28 +2686,28 @@
         <v>13</v>
       </c>
       <c r="C14" s="19">
-        <v>34228</v>
+        <v>35875</v>
       </c>
       <c r="D14" s="16">
-        <v>21685</v>
+        <v>22894</v>
       </c>
       <c r="E14" s="16">
-        <v>323</v>
+        <v>578</v>
       </c>
       <c r="F14" s="18">
-        <v>10062</v>
+        <v>10149</v>
       </c>
       <c r="G14" s="19">
-        <v>15961</v>
+        <v>16466</v>
       </c>
       <c r="H14" s="16">
-        <v>6232</v>
+        <v>6411</v>
       </c>
       <c r="I14" s="16">
         <v>0</v>
       </c>
       <c r="J14" s="18">
-        <v>7121</v>
+        <v>7573</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2729,28 +2718,28 @@
         <v>9</v>
       </c>
       <c r="C15" s="13">
-        <v>95415</v>
+        <v>99351</v>
       </c>
       <c r="D15" s="11">
-        <v>96391</v>
+        <v>98240</v>
       </c>
       <c r="E15" s="11">
-        <v>8918</v>
+        <v>9666</v>
       </c>
       <c r="F15" s="14">
         <v>33984</v>
       </c>
       <c r="G15" s="13">
-        <v>35408</v>
+        <v>36769</v>
       </c>
       <c r="H15" s="11">
-        <v>48249</v>
+        <v>49066</v>
       </c>
       <c r="I15" s="11">
-        <v>6799</v>
+        <v>6972</v>
       </c>
       <c r="J15" s="14">
-        <v>17938</v>
+        <v>18324</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2761,28 +2750,28 @@
         <v>10</v>
       </c>
       <c r="C16" s="19">
-        <v>42613</v>
+        <v>44712</v>
       </c>
       <c r="D16" s="16">
-        <v>52907</v>
+        <v>54693</v>
       </c>
       <c r="E16" s="16">
-        <v>4836</v>
+        <v>5074</v>
       </c>
       <c r="F16" s="18">
-        <v>30080</v>
+        <v>30382</v>
       </c>
       <c r="G16" s="19">
-        <v>21305</v>
+        <v>22374</v>
       </c>
       <c r="H16" s="16">
-        <v>28208</v>
+        <v>28970</v>
       </c>
       <c r="I16" s="16">
-        <v>2909</v>
+        <v>2921</v>
       </c>
       <c r="J16" s="18">
-        <v>17331</v>
+        <v>17929</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2793,28 +2782,28 @@
         <v>11</v>
       </c>
       <c r="C17" s="13">
-        <v>69485</v>
+        <v>72464</v>
       </c>
       <c r="D17" s="11">
-        <v>66650</v>
+        <v>69474</v>
       </c>
       <c r="E17" s="11">
-        <v>9654</v>
+        <v>9684</v>
       </c>
       <c r="F17" s="14">
-        <v>50719</v>
+        <v>50987</v>
       </c>
       <c r="G17" s="13">
-        <v>40174</v>
+        <v>40735</v>
       </c>
       <c r="H17" s="11">
-        <v>35535</v>
+        <v>35762</v>
       </c>
       <c r="I17" s="11">
-        <v>8769</v>
+        <v>8824</v>
       </c>
       <c r="J17" s="14">
-        <v>38703</v>
+        <v>39967</v>
       </c>
       <c r="K17" s="32"/>
     </row>
@@ -2826,96 +2815,88 @@
         <v>14</v>
       </c>
       <c r="C18" s="16">
-        <v>64309</v>
+        <v>65608</v>
       </c>
       <c r="D18" s="16">
-        <v>53394</v>
+        <v>53887</v>
       </c>
       <c r="E18" s="16">
-        <v>6193</v>
+        <v>6237</v>
       </c>
       <c r="F18" s="18">
-        <v>22616</v>
+        <v>22826</v>
       </c>
       <c r="G18" s="16">
-        <v>31644</v>
+        <v>33578</v>
       </c>
       <c r="H18" s="16">
-        <v>28161</v>
+        <v>28829</v>
       </c>
       <c r="I18" s="16">
-        <v>2912</v>
+        <v>3023</v>
       </c>
       <c r="J18" s="18">
-        <v>12272</v>
+        <v>12964</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="13">
-        <v>1898</v>
-      </c>
-      <c r="D19" s="11">
-        <v>1483</v>
-      </c>
-      <c r="E19" s="11">
-        <v>3</v>
-      </c>
-      <c r="F19" s="14">
-        <v>0</v>
-      </c>
-      <c r="G19" s="13">
-        <v>0</v>
-      </c>
-      <c r="H19" s="11">
-        <v>998</v>
-      </c>
-      <c r="I19" s="11">
-        <v>0</v>
-      </c>
-      <c r="J19" s="14">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="49" t="s">
+      <c r="A20" s="44"/>
+      <c r="B20" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="50">
-        <f t="shared" ref="C20:J20" si="0">SUM(C3:C19)</f>
-        <v>2004260</v>
-      </c>
-      <c r="D20" s="51">
-        <f t="shared" si="0"/>
-        <v>2008316</v>
-      </c>
-      <c r="E20" s="51">
-        <f t="shared" si="0"/>
-        <v>163215</v>
-      </c>
-      <c r="F20" s="52">
-        <f t="shared" si="0"/>
-        <v>827171</v>
-      </c>
-      <c r="G20" s="50">
-        <f t="shared" si="0"/>
-        <v>857467</v>
-      </c>
-      <c r="H20" s="51">
-        <f t="shared" si="0"/>
-        <v>1077525</v>
-      </c>
-      <c r="I20" s="51">
-        <f t="shared" si="0"/>
-        <v>85664</v>
-      </c>
-      <c r="J20" s="52">
-        <f t="shared" si="0"/>
-        <v>610545</v>
+      <c r="C20" s="49">
+        <v>2088744</v>
+      </c>
+      <c r="D20" s="50">
+        <v>2102436</v>
+      </c>
+      <c r="E20" s="50">
+        <v>176179</v>
+      </c>
+      <c r="F20" s="51">
+        <v>832726</v>
+      </c>
+      <c r="G20" s="49">
+        <v>899483</v>
+      </c>
+      <c r="H20" s="50">
+        <v>1102387</v>
+      </c>
+      <c r="I20" s="50">
+        <v>88545</v>
+      </c>
+      <c r="J20" s="51">
+        <v>623516</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2933,15 +2914,30 @@
         <v>43</v>
       </c>
     </row>
+    <row r="25" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+    </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -2955,9 +2951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926B42D2-7956-44E7-BD5B-5AF896796AC0}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2986,13 +2980,13 @@
         <v>44192</v>
       </c>
       <c r="B2" s="33">
-        <v>23555</v>
+        <v>23567</v>
       </c>
       <c r="C2" s="33">
         <v>0</v>
       </c>
       <c r="D2" s="33">
-        <v>23555</v>
+        <v>23567</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3000,13 +2994,13 @@
         <v>44193</v>
       </c>
       <c r="B3" s="33">
-        <v>18745</v>
+        <v>18746</v>
       </c>
       <c r="C3" s="33">
         <v>0</v>
       </c>
       <c r="D3" s="33">
-        <v>18745</v>
+        <v>18746</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3014,13 +3008,13 @@
         <v>44194</v>
       </c>
       <c r="B4" s="33">
-        <v>42579</v>
+        <v>42657</v>
       </c>
       <c r="C4" s="33">
         <v>0</v>
       </c>
       <c r="D4" s="33">
-        <v>42579</v>
+        <v>42657</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3028,13 +3022,13 @@
         <v>44195</v>
       </c>
       <c r="B5" s="33">
-        <v>57946</v>
+        <v>57997</v>
       </c>
       <c r="C5" s="33">
         <v>0</v>
       </c>
       <c r="D5" s="33">
-        <v>57946</v>
+        <v>57997</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3042,13 +3036,13 @@
         <v>44196</v>
       </c>
       <c r="B6" s="33">
-        <v>38621</v>
+        <v>38620</v>
       </c>
       <c r="C6" s="33">
         <v>0</v>
       </c>
       <c r="D6" s="33">
-        <v>38621</v>
+        <v>38620</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3070,13 +3064,13 @@
         <v>44198</v>
       </c>
       <c r="B8" s="33">
-        <v>51891</v>
+        <v>51975</v>
       </c>
       <c r="C8" s="33">
         <v>0</v>
       </c>
       <c r="D8" s="33">
-        <v>51891</v>
+        <v>51975</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3084,13 +3078,13 @@
         <v>44199</v>
       </c>
       <c r="B9" s="33">
-        <v>24990</v>
+        <v>24994</v>
       </c>
       <c r="C9" s="33">
         <v>0</v>
       </c>
       <c r="D9" s="33">
-        <v>24990</v>
+        <v>24994</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3126,13 +3120,13 @@
         <v>44202</v>
       </c>
       <c r="B12" s="33">
-        <v>58698</v>
+        <v>58674</v>
       </c>
       <c r="C12" s="33">
         <v>0</v>
       </c>
       <c r="D12" s="33">
-        <v>58698</v>
+        <v>58674</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3140,13 +3134,13 @@
         <v>44203</v>
       </c>
       <c r="B13" s="33">
-        <v>58403</v>
+        <v>58368</v>
       </c>
       <c r="C13" s="33">
         <v>0</v>
       </c>
       <c r="D13" s="33">
-        <v>58403</v>
+        <v>58368</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3154,13 +3148,13 @@
         <v>44204</v>
       </c>
       <c r="B14" s="33">
-        <v>60425</v>
+        <v>60383</v>
       </c>
       <c r="C14" s="33">
         <v>0</v>
       </c>
       <c r="D14" s="33">
-        <v>60425</v>
+        <v>60383</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3168,13 +3162,13 @@
         <v>44205</v>
       </c>
       <c r="B15" s="33">
-        <v>57236</v>
+        <v>57199</v>
       </c>
       <c r="C15" s="33">
         <v>0</v>
       </c>
       <c r="D15" s="33">
-        <v>57236</v>
+        <v>57199</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3196,13 +3190,13 @@
         <v>44207</v>
       </c>
       <c r="B17" s="33">
-        <v>65672</v>
+        <v>65591</v>
       </c>
       <c r="C17" s="33">
         <v>0</v>
       </c>
       <c r="D17" s="33">
-        <v>65672</v>
+        <v>65591</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3210,13 +3204,13 @@
         <v>44208</v>
       </c>
       <c r="B18" s="33">
-        <v>82140</v>
+        <v>82036</v>
       </c>
       <c r="C18" s="33">
         <v>0</v>
       </c>
       <c r="D18" s="33">
-        <v>82140</v>
+        <v>82036</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3224,13 +3218,13 @@
         <v>44209</v>
       </c>
       <c r="B19" s="33">
-        <v>99077</v>
+        <v>99012</v>
       </c>
       <c r="C19" s="33">
         <v>0</v>
       </c>
       <c r="D19" s="33">
-        <v>99077</v>
+        <v>99012</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3238,13 +3232,13 @@
         <v>44210</v>
       </c>
       <c r="B20" s="33">
-        <v>100054</v>
+        <v>100005</v>
       </c>
       <c r="C20" s="33">
         <v>114</v>
       </c>
       <c r="D20" s="33">
-        <v>100168</v>
+        <v>100119</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3252,13 +3246,13 @@
         <v>44211</v>
       </c>
       <c r="B21" s="33">
-        <v>92254</v>
+        <v>92253</v>
       </c>
       <c r="C21" s="33">
         <v>429</v>
       </c>
       <c r="D21" s="33">
-        <v>92683</v>
+        <v>92682</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3266,13 +3260,13 @@
         <v>44212</v>
       </c>
       <c r="B22" s="33">
-        <v>56716</v>
+        <v>56715</v>
       </c>
       <c r="C22" s="33">
         <v>397</v>
       </c>
       <c r="D22" s="33">
-        <v>57113</v>
+        <v>57112</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3294,13 +3288,13 @@
         <v>44214</v>
       </c>
       <c r="B24" s="33">
-        <v>57818</v>
+        <v>57816</v>
       </c>
       <c r="C24" s="33">
         <v>16410</v>
       </c>
       <c r="D24" s="33">
-        <v>74228</v>
+        <v>74226</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3308,13 +3302,13 @@
         <v>44215</v>
       </c>
       <c r="B25" s="33">
-        <v>67896</v>
+        <v>67893</v>
       </c>
       <c r="C25" s="33">
         <v>27231</v>
       </c>
       <c r="D25" s="33">
-        <v>95127</v>
+        <v>95124</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3322,13 +3316,13 @@
         <v>44216</v>
       </c>
       <c r="B26" s="33">
-        <v>78105</v>
+        <v>78101</v>
       </c>
       <c r="C26" s="33">
         <v>50654</v>
       </c>
       <c r="D26" s="33">
-        <v>128759</v>
+        <v>128755</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3336,13 +3330,13 @@
         <v>44217</v>
       </c>
       <c r="B27" s="33">
-        <v>60592</v>
+        <v>60545</v>
       </c>
       <c r="C27" s="33">
         <v>35434</v>
       </c>
       <c r="D27" s="33">
-        <v>96026</v>
+        <v>95979</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3350,13 +3344,13 @@
         <v>44218</v>
       </c>
       <c r="B28" s="33">
-        <v>84042</v>
+        <v>83988</v>
       </c>
       <c r="C28" s="33">
         <v>31289</v>
       </c>
       <c r="D28" s="33">
-        <v>115331</v>
+        <v>115277</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3364,13 +3358,13 @@
         <v>44219</v>
       </c>
       <c r="B29" s="33">
-        <v>48794</v>
+        <v>48795</v>
       </c>
       <c r="C29" s="33">
-        <v>43805</v>
+        <v>43851</v>
       </c>
       <c r="D29" s="33">
-        <v>92599</v>
+        <v>92646</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3378,13 +3372,13 @@
         <v>44220</v>
       </c>
       <c r="B30" s="33">
-        <v>38073</v>
+        <v>38067</v>
       </c>
       <c r="C30" s="33">
-        <v>28027</v>
+        <v>28150</v>
       </c>
       <c r="D30" s="33">
-        <v>66100</v>
+        <v>66217</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3392,13 +3386,13 @@
         <v>44221</v>
       </c>
       <c r="B31" s="33">
-        <v>57745</v>
+        <v>57744</v>
       </c>
       <c r="C31" s="33">
         <v>39594</v>
       </c>
       <c r="D31" s="33">
-        <v>97339</v>
+        <v>97338</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3409,10 +3403,10 @@
         <v>53109</v>
       </c>
       <c r="C32" s="33">
-        <v>49563</v>
+        <v>49578</v>
       </c>
       <c r="D32" s="33">
-        <v>102672</v>
+        <v>102687</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3423,10 +3417,10 @@
         <v>54022</v>
       </c>
       <c r="C33" s="33">
-        <v>58970</v>
+        <v>59096</v>
       </c>
       <c r="D33" s="33">
-        <v>112992</v>
+        <v>113118</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3434,13 +3428,13 @@
         <v>44224</v>
       </c>
       <c r="B34" s="33">
-        <v>51625</v>
+        <v>51580</v>
       </c>
       <c r="C34" s="33">
-        <v>48922</v>
+        <v>48850</v>
       </c>
       <c r="D34" s="33">
-        <v>100547</v>
+        <v>100430</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3448,13 +3442,13 @@
         <v>44225</v>
       </c>
       <c r="B35" s="33">
-        <v>55798</v>
+        <v>55801</v>
       </c>
       <c r="C35" s="33">
-        <v>53468</v>
+        <v>53401</v>
       </c>
       <c r="D35" s="33">
-        <v>109266</v>
+        <v>109202</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3462,13 +3456,13 @@
         <v>44226</v>
       </c>
       <c r="B36" s="33">
-        <v>39535</v>
+        <v>39542</v>
       </c>
       <c r="C36" s="33">
-        <v>47748</v>
+        <v>47821</v>
       </c>
       <c r="D36" s="33">
-        <v>87283</v>
+        <v>87363</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3476,13 +3470,13 @@
         <v>44227</v>
       </c>
       <c r="B37" s="33">
-        <v>31320</v>
+        <v>31331</v>
       </c>
       <c r="C37" s="33">
-        <v>31352</v>
+        <v>31381</v>
       </c>
       <c r="D37" s="33">
-        <v>62672</v>
+        <v>62712</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3490,13 +3484,13 @@
         <v>44228</v>
       </c>
       <c r="B38" s="33">
-        <v>49699</v>
+        <v>49700</v>
       </c>
       <c r="C38" s="33">
-        <v>65927</v>
+        <v>65858</v>
       </c>
       <c r="D38" s="33">
-        <v>115626</v>
+        <v>115558</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,13 +3498,13 @@
         <v>44229</v>
       </c>
       <c r="B39" s="33">
-        <v>57811</v>
+        <v>57830</v>
       </c>
       <c r="C39" s="33">
-        <v>69772</v>
+        <v>69726</v>
       </c>
       <c r="D39" s="33">
-        <v>127583</v>
+        <v>127556</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3518,13 +3512,13 @@
         <v>44230</v>
       </c>
       <c r="B40" s="33">
-        <v>57619</v>
+        <v>57618</v>
       </c>
       <c r="C40" s="33">
-        <v>84741</v>
+        <v>84562</v>
       </c>
       <c r="D40" s="33">
-        <v>142360</v>
+        <v>142180</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3532,13 +3526,13 @@
         <v>44231</v>
       </c>
       <c r="B41" s="33">
-        <v>62972</v>
+        <v>62920</v>
       </c>
       <c r="C41" s="33">
-        <v>72520</v>
+        <v>72438</v>
       </c>
       <c r="D41" s="33">
-        <v>135492</v>
+        <v>135358</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3546,13 +3540,13 @@
         <v>44232</v>
       </c>
       <c r="B42" s="33">
-        <v>59154</v>
+        <v>59148</v>
       </c>
       <c r="C42" s="33">
-        <v>72883</v>
+        <v>73036</v>
       </c>
       <c r="D42" s="33">
-        <v>132037</v>
+        <v>132184</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3560,13 +3554,13 @@
         <v>44233</v>
       </c>
       <c r="B43" s="33">
-        <v>48586</v>
+        <v>48589</v>
       </c>
       <c r="C43" s="33">
         <v>55159</v>
       </c>
       <c r="D43" s="33">
-        <v>103745</v>
+        <v>103748</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3574,13 +3568,13 @@
         <v>44234</v>
       </c>
       <c r="B44" s="33">
-        <v>32879</v>
+        <v>32880</v>
       </c>
       <c r="C44" s="33">
-        <v>26519</v>
+        <v>26520</v>
       </c>
       <c r="D44" s="33">
-        <v>59398</v>
+        <v>59400</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3588,13 +3582,13 @@
         <v>44235</v>
       </c>
       <c r="B45" s="33">
-        <v>55742</v>
+        <v>54663</v>
       </c>
       <c r="C45" s="33">
-        <v>51623</v>
+        <v>51584</v>
       </c>
       <c r="D45" s="33">
-        <v>107365</v>
+        <v>106247</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3602,13 +3596,13 @@
         <v>44236</v>
       </c>
       <c r="B46" s="33">
-        <v>59939</v>
+        <v>59520</v>
       </c>
       <c r="C46" s="33">
-        <v>64760</v>
+        <v>64962</v>
       </c>
       <c r="D46" s="33">
-        <v>124699</v>
+        <v>124482</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3616,13 +3610,13 @@
         <v>44237</v>
       </c>
       <c r="B47" s="33">
-        <v>74965</v>
+        <v>74900</v>
       </c>
       <c r="C47" s="33">
-        <v>74201</v>
+        <v>74157</v>
       </c>
       <c r="D47" s="33">
-        <v>149166</v>
+        <v>149057</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3630,13 +3624,13 @@
         <v>44238</v>
       </c>
       <c r="B48" s="33">
-        <v>71206</v>
+        <v>71275</v>
       </c>
       <c r="C48" s="33">
-        <v>72412</v>
+        <v>72411</v>
       </c>
       <c r="D48" s="33">
-        <v>143618</v>
+        <v>143686</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3644,13 +3638,13 @@
         <v>44239</v>
       </c>
       <c r="B49" s="33">
-        <v>79752</v>
+        <v>79798</v>
       </c>
       <c r="C49" s="33">
-        <v>78008</v>
+        <v>77910</v>
       </c>
       <c r="D49" s="33">
-        <v>157760</v>
+        <v>157708</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,13 +3652,13 @@
         <v>44240</v>
       </c>
       <c r="B50" s="33">
-        <v>63233</v>
+        <v>63234</v>
       </c>
       <c r="C50" s="33">
         <v>46624</v>
       </c>
       <c r="D50" s="33">
-        <v>109857</v>
+        <v>109858</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3675,10 +3669,10 @@
         <v>39778</v>
       </c>
       <c r="C51" s="33">
-        <v>26985</v>
+        <v>26984</v>
       </c>
       <c r="D51" s="33">
-        <v>66763</v>
+        <v>66762</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3686,13 +3680,13 @@
         <v>44242</v>
       </c>
       <c r="B52" s="33">
-        <v>70751</v>
+        <v>70744</v>
       </c>
       <c r="C52" s="33">
-        <v>56025</v>
+        <v>56029</v>
       </c>
       <c r="D52" s="33">
-        <v>126776</v>
+        <v>126773</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3700,13 +3694,13 @@
         <v>44243</v>
       </c>
       <c r="B53" s="33">
-        <v>81375</v>
+        <v>81394</v>
       </c>
       <c r="C53" s="33">
-        <v>54744</v>
+        <v>54756</v>
       </c>
       <c r="D53" s="33">
-        <v>136119</v>
+        <v>136150</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3714,13 +3708,13 @@
         <v>44244</v>
       </c>
       <c r="B54" s="33">
-        <v>94295</v>
+        <v>94139</v>
       </c>
       <c r="C54" s="33">
         <v>54620</v>
       </c>
       <c r="D54" s="33">
-        <v>148915</v>
+        <v>148759</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3728,13 +3722,13 @@
         <v>44245</v>
       </c>
       <c r="B55" s="33">
-        <v>92926</v>
+        <v>93086</v>
       </c>
       <c r="C55" s="33">
-        <v>52025</v>
+        <v>52037</v>
       </c>
       <c r="D55" s="33">
-        <v>144951</v>
+        <v>145123</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3742,13 +3736,13 @@
         <v>44246</v>
       </c>
       <c r="B56" s="33">
-        <v>96504</v>
+        <v>96546</v>
       </c>
       <c r="C56" s="33">
-        <v>53532</v>
+        <v>53485</v>
       </c>
       <c r="D56" s="33">
-        <v>150036</v>
+        <v>150031</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3756,13 +3750,13 @@
         <v>44247</v>
       </c>
       <c r="B57" s="33">
-        <v>74887</v>
+        <v>74896</v>
       </c>
       <c r="C57" s="33">
         <v>37611</v>
       </c>
       <c r="D57" s="33">
-        <v>112498</v>
+        <v>112507</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3770,13 +3764,13 @@
         <v>44248</v>
       </c>
       <c r="B58" s="33">
-        <v>56650</v>
+        <v>56649</v>
       </c>
       <c r="C58" s="33">
         <v>28943</v>
       </c>
       <c r="D58" s="33">
-        <v>85593</v>
+        <v>85592</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3784,13 +3778,13 @@
         <v>44249</v>
       </c>
       <c r="B59" s="33">
-        <v>99061</v>
+        <v>98885</v>
       </c>
       <c r="C59" s="33">
-        <v>52640</v>
+        <v>52642</v>
       </c>
       <c r="D59" s="33">
-        <v>151701</v>
+        <v>151527</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3798,13 +3792,13 @@
         <v>44250</v>
       </c>
       <c r="B60" s="33">
-        <v>103698</v>
+        <v>103514</v>
       </c>
       <c r="C60" s="33">
-        <v>55370</v>
+        <v>55379</v>
       </c>
       <c r="D60" s="33">
-        <v>159068</v>
+        <v>158893</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3812,13 +3806,13 @@
         <v>44251</v>
       </c>
       <c r="B61" s="33">
-        <v>115987</v>
+        <v>116106</v>
       </c>
       <c r="C61" s="33">
-        <v>57423</v>
+        <v>57431</v>
       </c>
       <c r="D61" s="33">
-        <v>173410</v>
+        <v>173537</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3826,13 +3820,13 @@
         <v>44252</v>
       </c>
       <c r="B62" s="33">
-        <v>126264</v>
+        <v>126573</v>
       </c>
       <c r="C62" s="33">
-        <v>51504</v>
+        <v>51528</v>
       </c>
       <c r="D62" s="33">
-        <v>177768</v>
+        <v>178101</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3840,83 +3834,97 @@
         <v>44253</v>
       </c>
       <c r="B63" s="33">
-        <v>132766</v>
+        <v>134077</v>
       </c>
       <c r="C63" s="33">
-        <v>57468</v>
+        <v>57793</v>
       </c>
       <c r="D63" s="33">
-        <v>190234</v>
+        <v>191870</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="38">
         <v>44254</v>
       </c>
-      <c r="B64" s="44">
-        <v>106896</v>
-      </c>
-      <c r="C64" s="44">
-        <v>38515</v>
-      </c>
-      <c r="D64" s="44">
-        <v>145411</v>
+      <c r="B64" s="33">
+        <v>107277</v>
+      </c>
+      <c r="C64" s="33">
+        <v>38506</v>
+      </c>
+      <c r="D64" s="33">
+        <v>145783</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="38">
         <v>44255</v>
       </c>
-      <c r="B65" s="44">
-        <v>85568</v>
-      </c>
-      <c r="C65" s="44">
-        <v>27653</v>
-      </c>
-      <c r="D65" s="44">
-        <v>113221</v>
+      <c r="B65" s="33">
+        <v>85595</v>
+      </c>
+      <c r="C65" s="33">
+        <v>27748</v>
+      </c>
+      <c r="D65" s="33">
+        <v>113343</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="38">
         <v>44256</v>
       </c>
-      <c r="B66" s="44">
-        <v>138451</v>
-      </c>
-      <c r="C66" s="44">
-        <v>49291</v>
-      </c>
-      <c r="D66" s="44">
-        <v>187742</v>
+      <c r="B66" s="33">
+        <v>139231</v>
+      </c>
+      <c r="C66" s="33">
+        <v>49515</v>
+      </c>
+      <c r="D66" s="33">
+        <v>188746</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="38">
         <v>44257</v>
       </c>
-      <c r="B67" s="44">
-        <v>153763</v>
-      </c>
-      <c r="C67" s="44">
-        <v>54331</v>
-      </c>
-      <c r="D67" s="44">
-        <v>208094</v>
+      <c r="B67" s="33">
+        <v>154406</v>
+      </c>
+      <c r="C67" s="33">
+        <v>55072</v>
+      </c>
+      <c r="D67" s="33">
+        <v>209478</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="38">
         <v>44258</v>
       </c>
-      <c r="B68">
-        <v>140754</v>
-      </c>
-      <c r="C68">
-        <v>50938</v>
-      </c>
-      <c r="D68">
-        <v>191692</v>
+      <c r="B68" s="33">
+        <v>167225</v>
+      </c>
+      <c r="C68" s="33">
+        <v>65219</v>
+      </c>
+      <c r="D68" s="33">
+        <v>232444</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="38">
+        <v>44259</v>
+      </c>
+      <c r="B69" s="33">
+        <v>166870</v>
+      </c>
+      <c r="C69" s="33">
+        <v>58853</v>
+      </c>
+      <c r="D69" s="33">
+        <v>225723</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3925,15 +3933,15 @@
       </c>
       <c r="B72" s="33">
         <f>SUM(B2:B71)</f>
-        <v>4541389</v>
+        <v>4736174</v>
       </c>
       <c r="C72" s="33">
         <f t="shared" ref="C72" si="0">SUM(C2:C71)</f>
-        <v>2271784</v>
+        <v>2346388</v>
       </c>
       <c r="D72" s="33">
         <f>SUM(D2:D71)</f>
-        <v>6813173</v>
+        <v>7082562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>